<commit_message>
Fixed onko_kimppa check, removed some comments
Fixed onko_kimppa check.
Removed some comments.
</commit_message>
<xml_diff>
--- a/tests/data/test_kompostori/ilmoitukset.xlsx
+++ b/tests/data/test_kompostori/ilmoitukset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="142">
   <si>
     <t xml:space="preserve">Vastausaika</t>
   </si>
@@ -292,6 +292,9 @@
     <t xml:space="preserve">Elokuu</t>
   </si>
   <si>
+    <t xml:space="preserve">Kompostori on useamman kiinteistön yhteinen kompostori (voit ilmoittaa enintään 5 rakennusta)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hyväksytty</t>
   </si>
   <si>
@@ -391,6 +394,9 @@
     <t xml:space="preserve">Joulukuu</t>
   </si>
   <si>
+    <t xml:space="preserve">Kompostoria käyttää yksi rakennus, joka on ilmoitettu yllä Kompostorin sijainti -kohdassa</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yksittäinen</t>
   </si>
   <si>
@@ -433,25 +439,7 @@
     <t xml:space="preserve">0500654321</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">hylätty.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">henri@suomi.fi</t>
-    </r>
+    <t xml:space="preserve">hylätty.henri@suomi.fi</t>
   </si>
   <si>
     <t xml:space="preserve">134567890C</t>
@@ -469,7 +457,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -517,11 +505,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -584,7 +567,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -634,10 +617,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -767,8 +746,8 @@
   </sheetPr>
   <dimension ref="A1:BT6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BC1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BT10" activeCellId="0" sqref="BT10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AO27" activeCellId="0" sqref="AO27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1107,8 +1086,8 @@
       <c r="AQ2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AV2" s="1" t="n">
-        <v>2</v>
+      <c r="AV2" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="AW2" s="1" t="s">
         <v>75</v>
@@ -1135,19 +1114,19 @@
         <v>83</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BF2" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BQ2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BR2" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BT2" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,109 +1229,109 @@
       <c r="AQ3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AV3" s="1" t="n">
-        <v>2</v>
+      <c r="AV3" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AY3" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AZ3" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="BA3" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="BB3" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BC3" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BD3" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BE3" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BF3" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BQ3" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BR3" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BT3" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="R4" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y4" s="1" t="n">
         <v>5</v>
@@ -1373,25 +1352,25 @@
         <v>86</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AI4" s="1" t="n">
         <v>12</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AO4" s="1" t="s">
         <v>87</v>
@@ -1403,63 +1382,63 @@
         <v>89</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AV4" s="1" t="n">
-        <v>1</v>
+        <v>123</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="AW4" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AX4" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AY4" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AZ4" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="BA4" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="BB4" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="BC4" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="BD4" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="BE4" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BF4" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="BQ4" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BR4" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BT4" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>73</v>
@@ -1468,55 +1447,55 @@
         <v>74</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="O5" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="Q5" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>84</v>
@@ -1546,19 +1525,19 @@
         <v>12</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AL5" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AM5" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AO5" s="1" t="s">
         <v>87</v>
@@ -1570,81 +1549,81 @@
         <v>89</v>
       </c>
       <c r="AR5" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AS5" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AV5" s="1" t="n">
-        <v>1</v>
+        <v>123</v>
+      </c>
+      <c r="AV5" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="AW5" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AY5" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AZ5" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="BA5" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="BB5" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="BC5" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="BD5" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="BE5" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BF5" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BQ5" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BR5" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BT5" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>139</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>79</v>
@@ -1655,117 +1634,117 @@
       <c r="J6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N6" s="0" t="s">
-        <v>134</v>
+      <c r="N6" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="P6" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>79</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="R6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="S6" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="T6" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="U6" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="V6" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="W6" s="0" t="s">
+      <c r="S6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="W6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Y6" s="0" t="n">
+      <c r="Y6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Z6" s="0" t="n">
+      <c r="Z6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AA6" s="0" t="n">
+      <c r="AA6" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="AD6" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="AF6" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG6" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH6" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="AI6" s="0" t="n">
+      <c r="AD6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AJ6" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="AK6" s="0" t="s">
+      <c r="AJ6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AV6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW6" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="AX6" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="AY6" s="0" t="s">
+      <c r="AK6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AV6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AW6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AX6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY6" s="1" t="s">
         <v>79</v>
       </c>
       <c r="AZ6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="BA6" s="0" t="s">
+      <c r="BA6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BB6" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="BC6" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="BD6" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="BE6" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="BF6" s="0" t="s">
+      <c r="BB6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="BC6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="BD6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="BE6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BQ6" s="0" t="s">
-        <v>91</v>
+      <c r="BQ6" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="BR6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="BT6" s="0" t="s">
-        <v>135</v>
+        <v>93</v>
+      </c>
+      <c r="BT6" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" display="tytti@laulumuisto.fi"/>
     <hyperlink ref="G5" r:id="rId2" display="keke.kohdentumaton@email.fi"/>
-    <hyperlink ref="G6" r:id="rId3" display="henri@suomi.fi"/>
+    <hyperlink ref="G6" r:id="rId3" display="hylätty.henri@suomi.fi"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added kohdennus for ilmoituksen vastuuhenkilo.
- Read Kompostori location prt.
- Added find_osoite_by_prt to buildings.py
- Added ioptional parameter to find_kohde_by_prt, to use sijainti_prt for finding kohde.
- Added kohdennus for ilmoituksen vastuuhenkilo.
- Added selecting osoite_id from Kompostorin sijainti building.
</commit_message>
<xml_diff>
--- a/tests/data/test_kompostori/ilmoitukset.xlsx
+++ b/tests/data/test_kompostori/ilmoitukset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="143">
   <si>
     <t xml:space="preserve">Vastausaika</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t xml:space="preserve">100456700C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100456700C, 100456700D</t>
   </si>
   <si>
     <t xml:space="preserve">15.1.2022</t>
@@ -457,7 +460,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -504,13 +507,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -567,7 +563,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -613,10 +609,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -746,8 +738,8 @@
   </sheetPr>
   <dimension ref="A1:BT6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO27" activeCellId="0" sqref="AO27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1492,7 +1484,7 @@
         <v>134</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>134</v>
@@ -1605,7 +1597,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>73</v>
@@ -1614,16 +1606,16 @@
         <v>74</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="12" t="s">
         <v>139</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>79</v>
@@ -1638,10 +1630,10 @@
         <v>81</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>79</v>
@@ -1653,16 +1645,16 @@
         <v>81</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>84</v>
@@ -1677,7 +1669,7 @@
         <v>60</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>114</v>
@@ -1701,10 +1693,10 @@
         <v>124</v>
       </c>
       <c r="AW6" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AY6" s="1" t="s">
         <v>79</v>
@@ -1716,16 +1708,16 @@
         <v>81</v>
       </c>
       <c r="BB6" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BC6" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BD6" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="BE6" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="BF6" s="1" t="s">
         <v>84</v>
@@ -1737,7 +1729,7 @@
         <v>93</v>
       </c>
       <c r="BT6" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added kohdentumaton kimppa to test data. Added test for kohdentumattomat.
Various fixes after rebase.
</commit_message>
<xml_diff>
--- a/tests/data/test_kompostori/ilmoitukset.xlsx
+++ b/tests/data/test_kompostori/ilmoitukset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="154">
   <si>
     <t xml:space="preserve">Vastausaika</t>
   </si>
@@ -301,9 +301,6 @@
     <t xml:space="preserve">Käsitelty</t>
   </si>
   <si>
-    <t xml:space="preserve">2027-01-11 00:00:00</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kimppa</t>
   </si>
   <si>
@@ -449,6 +446,42 @@
   </si>
   <si>
     <t xml:space="preserve">KekkiläKomposti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.1.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026.1.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virheellinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.1.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2027-01-11 2:43:10.477000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kohdentumaton kimppa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apumies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apumiehentie 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">125456766A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2027-01-28 2:43:10.477000</t>
   </si>
 </sst>
 </file>
@@ -736,10 +769,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT6"/>
+  <dimension ref="A1:BT9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BP18" activeCellId="0" sqref="BP18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -757,7 +790,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="52" min="52" style="2" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="64" style="2" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="70" min="70" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="3" width="17.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,11 +1147,11 @@
       <c r="BQ2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BR2" s="8" t="s">
+      <c r="BR2" s="8" t="n">
+        <v>46398.0000034722</v>
+      </c>
+      <c r="BT2" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="BT2" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,28 +1258,28 @@
         <v>90</v>
       </c>
       <c r="AW3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX3" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AX3" s="1" t="s">
+      <c r="AY3" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="AY3" s="7" t="s">
+      <c r="AZ3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AZ3" s="2" t="s">
+      <c r="BA3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="BA3" s="1" t="s">
+      <c r="BB3" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="BB3" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="BC3" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BD3" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BE3" s="1" t="s">
         <v>91</v>
@@ -1257,73 +1290,73 @@
       <c r="BQ3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BR3" s="8" t="s">
+      <c r="BR3" s="8" t="n">
+        <v>46398</v>
+      </c>
+      <c r="BT3" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="BT3" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S4" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S4" s="7" t="s">
+      <c r="T4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="Y4" s="1" t="n">
         <v>5</v>
@@ -1344,25 +1377,25 @@
         <v>86</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AI4" s="1" t="n">
         <v>12</v>
       </c>
       <c r="AJ4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AL4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AM4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="AO4" s="1" t="s">
         <v>87</v>
@@ -1374,63 +1407,63 @@
         <v>89</v>
       </c>
       <c r="AR4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS4" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AT4" s="1" t="s">
+      <c r="AU4" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AU4" s="1" t="s">
+      <c r="AV4" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AV4" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="AW4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX4" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="AX4" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="AY4" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BB4" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="AZ4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="BA4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BB4" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="BC4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BD4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BE4" s="1" t="s">
         <v>91</v>
       </c>
       <c r="BF4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BQ4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BR4" s="8" t="s">
-        <v>93</v>
+      <c r="BR4" s="8" t="n">
+        <v>46398.0000011574</v>
       </c>
       <c r="BT4" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>73</v>
@@ -1439,55 +1472,55 @@
         <v>74</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="U5" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="V5" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="V5" s="7" t="s">
-        <v>134</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>84</v>
@@ -1517,19 +1550,19 @@
         <v>12</v>
       </c>
       <c r="AJ5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AK5" s="1" t="s">
+      <c r="AL5" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AL5" s="11" t="s">
+      <c r="AM5" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="AM5" s="11" t="s">
+      <c r="AN5" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="AO5" s="1" t="s">
         <v>87</v>
@@ -1541,43 +1574,43 @@
         <v>89</v>
       </c>
       <c r="AR5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AS5" s="1" t="s">
+      <c r="AT5" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AT5" s="1" t="s">
+      <c r="AU5" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AU5" s="1" t="s">
+      <c r="AV5" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AV5" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="AW5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AX5" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="AY5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AZ5" s="2" t="s">
+      <c r="BA5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="BA5" s="1" t="s">
+      <c r="BB5" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="BB5" s="7" t="s">
-        <v>134</v>
-      </c>
       <c r="BC5" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BD5" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BE5" s="1" t="s">
         <v>91</v>
@@ -1588,16 +1621,16 @@
       <c r="BQ5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BR5" s="8" t="s">
-        <v>93</v>
+      <c r="BR5" s="8" t="n">
+        <v>46398</v>
       </c>
       <c r="BT5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>73</v>
@@ -1606,16 +1639,16 @@
         <v>74</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="10" t="s">
         <v>139</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>140</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>79</v>
@@ -1630,10 +1663,10 @@
         <v>81</v>
       </c>
       <c r="N6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>79</v>
@@ -1645,16 +1678,16 @@
         <v>81</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>84</v>
@@ -1669,34 +1702,34 @@
         <v>60</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AI6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AJ6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AK6" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="AV6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AW6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AX6" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="AX6" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="AY6" s="1" t="s">
         <v>79</v>
@@ -1708,16 +1741,16 @@
         <v>81</v>
       </c>
       <c r="BB6" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC6" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BD6" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BE6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BF6" s="1" t="s">
         <v>84</v>
@@ -1725,11 +1758,482 @@
       <c r="BQ6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BR6" s="3" t="s">
-        <v>93</v>
+      <c r="BR6" s="3" t="n">
+        <v>46398</v>
       </c>
       <c r="BT6" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>138</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AV7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AW7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AX7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB7" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="BC7" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="BD7" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="BE7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BR7" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="BT7" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="V8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI8" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL8" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="AM8" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AT8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AU8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AV8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="BA8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BB8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="BC8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="BD8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="BE8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BR8" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="BT8" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="V9" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI9" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL9" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="AM9" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR9" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AT9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AZ9" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="BA9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BB9" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BC9" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BD9" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BE9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BR9" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT9" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1737,6 +2241,9 @@
     <hyperlink ref="G4" r:id="rId1" display="tytti@laulumuisto.fi"/>
     <hyperlink ref="G5" r:id="rId2" display="keke.kohdentumaton@email.fi"/>
     <hyperlink ref="G6" r:id="rId3" display="hylätty.henri@suomi.fi"/>
+    <hyperlink ref="G7" r:id="rId4" display="hylätty.henri@suomi.fi"/>
+    <hyperlink ref="G8" r:id="rId5" display="keke.kohdentumaton@email.fi"/>
+    <hyperlink ref="G9" r:id="rId6" display="keke.kohdentumaton@email.fi"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Block emtry etunimi and sukunimi combination.
- Added validator that makes sure each vastuuhenkilo and kompostoija have either etu- or sukunimi.
- Modified test data to include one row with empty etu- and sukunimi.
</commit_message>
<xml_diff>
--- a/tests/data/test_kompostori/ilmoitukset.xlsx
+++ b/tests/data/test_kompostori/ilmoitukset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="155">
   <si>
     <t xml:space="preserve">Vastausaika</t>
   </si>
@@ -476,6 +476,15 @@
   </si>
   <si>
     <t xml:space="preserve">2027-01-28 2:43:10.477000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.1.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tytti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuntematon</t>
   </si>
 </sst>
 </file>
@@ -763,10 +772,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT9"/>
+  <dimension ref="A1:BT10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="10:10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2228,6 +2237,164 @@
         <v>145</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="V10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI10" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AT10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AX10" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AY10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BB10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="BC10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="BD10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="BE10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BQ10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BR10" s="8" t="n">
+        <v>46416</v>
+      </c>
+      <c r="BT10" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" display="tytti@laulumuisto.fi"/>
@@ -2236,6 +2403,7 @@
     <hyperlink ref="G7" r:id="rId4" display="hylätty.henri@suomi.fi"/>
     <hyperlink ref="G8" r:id="rId5" display="keke.kohdentumaton@email.fi"/>
     <hyperlink ref="G9" r:id="rId6" display="keke.kohdentumaton@email.fi"/>
+    <hyperlink ref="G10" r:id="rId7" display="tytti@laulumuisto.fi"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Korjattu testidatassa käytetty sarakkeen nimi
</commit_message>
<xml_diff>
--- a/tests/data/test_kompostori/ilmoitukset.xlsx
+++ b/tests/data/test_kompostori/ilmoitukset.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">Kompostorin käyttökuukaudet kalenterivuoden aikana:Joulukuu</t>
   </si>
   <si>
-    <t xml:space="preserve">Kompostoria käyttävien rakennusten lukumäärä</t>
+    <t xml:space="preserve">Kompostoria käyttävien asuinhuoneistojen lukumäärä</t>
   </si>
   <si>
     <t xml:space="preserve">1. Kompostoria käyttävän rakennuksen tiedot:Haltijan etunimi</t>
@@ -527,7 +527,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -661,133 +661,27 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BT10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="10:10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AP5" activeCellId="0" sqref="AP5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="47.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="48.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="48.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="53.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="49.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="50.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="51.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="51.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="54.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="57.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.53"/>

</xml_diff>